<commit_message>
fix: Rerun Histology metadata reharmonization procedure
</commit_message>
<xml_diff>
--- a/metadata/histology/todo/Vanderbilt TMC (Histology).xlsx
+++ b/metadata/histology/todo/Vanderbilt TMC (Histology).xlsx
@@ -13,7 +13,6 @@
     <sheet name="Invalid Input Pattern" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Non-Standard Value'!$A$1:$E$78</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Missing Required Value'!$A$1:$D$331</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Invalid Input Pattern'!$A$1:$F$80</definedName>
   </definedNames>
@@ -420,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,11 +440,6 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
           <t>hour</t>
         </is>
       </c>
@@ -463,31 +457,26 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
           <t>month</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="D3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>year</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="D4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>day</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="D5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>minute</t>
         </is>
@@ -504,7 +493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,1784 +528,7 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>HBM227.THVC.544</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM227.THVC.544</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>HBM264.XSVF.528</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM264.XSVF.528</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>HBM276.PGFS.693</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM276.PGFS.693</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>HBM296.RLWW.755</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM296.RLWW.755</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>HBM297.RSTP.985</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM297.RSTP.985</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>HBM324.MKTZ.248</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM324.MKTZ.248</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>HBM324.ZGZM.874</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM324.ZGZM.874</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>HBM325.RVSR.229</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM325.RVSR.229</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>HBM337.ZVPK.369</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM337.ZVPK.369</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>HBM338.RFPS.979</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM338.RFPS.979</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>HBM344.LLLV.539</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM344.LLLV.539</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>HBM346.WRZP.637</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM346.WRZP.637</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>HBM362.PTQJ.743</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM362.PTQJ.743</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>HBM389.KJJP.875</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM389.KJJP.875</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>HBM389.MBWW.346</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM389.MBWW.346</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>HBM396.KGDR.538</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM396.KGDR.538</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>HBM396.XMSB.623</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM396.XMSB.623</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>HBM428.QSKJ.486</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM428.QSKJ.486</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>HBM463.JRTB.582</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM463.JRTB.582</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>HBM473.FKKH.583</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM473.FKKH.583</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>HBM484.RDZR.494</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM484.RDZR.494</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>HBM486.KPCH.364</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM486.KPCH.364</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>HBM528.QSDN.323</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM528.QSDN.323</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>HBM535.BDNV.724</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM535.BDNV.724</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>HBM538.XVLP.889</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM538.XVLP.889</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>HBM593.DVGN.469</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM593.DVGN.469</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>HBM594.SRGW.833</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM594.SRGW.833</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>HBM623.BNWW.574</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM623.BNWW.574</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>HBM623.RPMC.638</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM623.RPMC.638</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>HBM627.RSGW.898</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM627.RSGW.898</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>HBM635.BSPV.599</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM635.BSPV.599</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>HBM636.GVWP.354</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM636.GVWP.354</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>HBM636.ZPTS.368</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM636.ZPTS.368</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>HBM649.DLZF.463</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM649.DLZF.463</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>HBM649.XFQG.775</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM649.XFQG.775</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>HBM653.BLLX.289</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr"/>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM653.BLLX.289</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>HBM654.GRHB.837</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr"/>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM654.GRHB.837</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>HBM655.VSLD.867</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM655.VSLD.867</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>HBM662.PMPZ.644</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr"/>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM662.PMPZ.644</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>HBM673.JJRZ.435</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM673.JJRZ.435</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>HBM676.SNVK.793</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM676.SNVK.793</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>HBM685.HZFG.838</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM685.HZFG.838</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>HBM725.PDDC.788</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM725.PDDC.788</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>HBM738.MXDD.328</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM738.MXDD.328</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>HBM745.BCRF.958</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM745.BCRF.958</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>HBM759.LQKN.226</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr"/>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM759.LQKN.226</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>HBM783.GDKK.879</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr"/>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM783.GDKK.879</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>HBM783.GJWP.694</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr"/>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM783.GJWP.694</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>HBM796.FZWQ.899</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr"/>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM796.FZWQ.899</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>HBM832.FQKR.463</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr"/>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM832.FQKR.463</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>HBM833.DBGG.252</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr"/>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM833.DBGG.252</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>HBM836.VTFP.364</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr"/>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM836.VTFP.364</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>HBM837.XGBD.427</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr"/>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM837.XGBD.427</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>HBM838.HGWL.498</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr"/>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM838.HGWL.498</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>HBM846.FTPG.677</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr"/>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM846.FTPG.677</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>HBM849.XMPC.398</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM849.XMPC.398</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>HBM852.NQRZ.779</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr"/>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM852.NQRZ.779</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>HBM864.MFDZ.983</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr"/>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM864.MFDZ.983</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>HBM872.HWNB.835</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr"/>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM872.HWNB.835</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>HBM874.RZDW.757</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr"/>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM874.RZDW.757</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>HBM875.QHDJ.259</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr"/>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM875.QHDJ.259</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>HBM879.CDHB.995</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr"/>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM879.CDHB.995</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>HBM884.QGXZ.934</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr"/>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM884.QGXZ.934</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>HBM885.XWNH.985</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr"/>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM885.XWNH.985</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>HBM892.SQNT.843</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr"/>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM892.SQNT.843</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>HBM937.TDGJ.774</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr"/>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM937.TDGJ.774</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>HBM939.TZWB.238</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr"/>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM939.TZWB.238</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>HBM947.VKMP.764</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr"/>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM947.VKMP.764</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>HBM957.LDNV.942</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr"/>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM957.LDNV.942</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>HBM958.GHFM.676</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr"/>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM958.GHFM.676</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>HBM964.CZLM.657</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr"/>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM964.CZLM.657</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>HBM969.MLWK.466</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr"/>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM969.MLWK.466</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>HBM977.RFWJ.484</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr"/>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM977.RFWJ.484</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>HBM978.CGGC.988</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr"/>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM978.CGGC.988</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>HBM979.HDZH.896</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr"/>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM979.HDZH.896</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>HBM984.PMZN.942</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr"/>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM984.PMZN.942</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>HBM987.NCDW.845</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>is_staining_automated</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr"/>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>https://portal.hubmapconsortium.org/browse/HBM987.NCDW.845</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E78"/>
-  <dataValidations count="1">
-    <dataValidation sqref="D2 D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31 D32 D33 D34 D35 D36 D37 D38 D39 D40 D41 D42 D43 D44 D45 D46 D47 D48 D49 D50 D51 D52 D53 D54 D55 D56 D57 D58 D59 D60 D61 D62 D63 D64 D65 D66 D67 D68 D69 D70 D71 D72 D73 D74 D75 D76 D77 D78" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
-      <formula1>_validation_data!$C$1:$C$2</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -8307,7 +6519,7 @@
       <formula1>_validation_data!$B$1:$B$2</formula1>
     </dataValidation>
     <dataValidation sqref="C4 C9 C14 C18 C22 C26 C30 C34 C38 C42 C46 C50 C55 C59 C64 C69 C73 C77 C82 C87 C91 C95 C99 C103 C107 C111 C115 C119 C124 C128 C132 C137 C142 C146 C150 C154 C158 C162 C167 C171 C176 C180 C185 C189 C193 C197 C202 C207 C211 C215 C220 C224 C228 C232 C236 C241 C245 C249 C253 C258 C263 C268 C272 C276 C280 C284 C288 C292 C296 C301 C305 C309 C313 C317 C322 C326 C330" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Your entry is not in the list" promptTitle="List Selection" prompt="Please select from the list" type="list">
-      <formula1>_validation_data!$D$1:$D$5</formula1>
+      <formula1>_validation_data!$C$1:$C$5</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>